<commit_message>
Charts four to six
No title yet
</commit_message>
<xml_diff>
--- a/public/support files/unique-charts.xlsx
+++ b/public/support files/unique-charts.xlsx
@@ -1444,7 +1444,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1533,11 +1533,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
@@ -1551,11 +1551,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">

</xml_diff>